<commit_message>
update questions y test view
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="categories" sheetId="1" r:id="rId5"/>
     <sheet state="visible" name="questions" sheetId="2" r:id="rId6"/>
     <sheet state="visible" name="tests" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="version" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
   <si>
     <t>Categoría</t>
   </si>
@@ -51,61 +52,61 @@
     <t>¿Cuántos granos de arroz hay en el típico paquete de arroz de 1 kilo?</t>
   </si>
   <si>
-    <t>¿Cuántas latas de CocaCola se beberán hoy en España?</t>
-  </si>
-  <si>
-    <t>¿Cuántos McDonald hay en España?</t>
-  </si>
-  <si>
-    <t>¿Cuántos afinadores de piano hay en España?</t>
-  </si>
-  <si>
-    <t>¿Cuántas veces late tu corazón durante una clase de lengua de una hora?</t>
-  </si>
-  <si>
-    <t>¿Cada cuántos segundos despega un avión en Barajas?</t>
-  </si>
-  <si>
-    <t>¿Cuántas búsquedas de Google se hacen por segundo?</t>
-  </si>
-  <si>
-    <t>¿Cuántos gente entra al metro cada minuto en Madrid a las 7am?</t>
-  </si>
-  <si>
-    <t>1 de cada ___ seres humanos en el mundo es profesor de instituto (12 - 18 años)</t>
-  </si>
-  <si>
-    <t>1 de cada ___ seres humanos en el mundo es profesor de instituto y asturiano</t>
-  </si>
-  <si>
-    <t>1 de cada ___ seres humanos en el mundo es chino, informático profesional y zurdo</t>
-  </si>
-  <si>
-    <t>1 de cada ___ españoles es pelirrojo, peluquero, zurdo y murciano</t>
-  </si>
-  <si>
-    <t>¿Cuántas horas dormirás el año que viene?</t>
-  </si>
-  <si>
-    <t>¿Cuántas horas duró la 2a Guerra Mundial?</t>
-  </si>
-  <si>
-    <t>¿Cuántos días tardas andando a Moscú?</t>
+    <t>¿Cuántas lentejas caben en una bañera?</t>
+  </si>
+  <si>
+    <t>¿Cuántos spaguetis caben en el contenedor de un típico camión de los grandes que vemos en la carretera?</t>
+  </si>
+  <si>
+    <t>¿Cuántos garbanzos caben en una piscina olímpica?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces late tu corazón durante una hora?</t>
+  </si>
+  <si>
+    <t>¿Cuántas búsquedas de Google se hacen al día en España?</t>
+  </si>
+  <si>
+    <t>¿Cuántos cafés se beben en Europa un lunes?</t>
+  </si>
+  <si>
+    <t>¿Cuántas respiraciones han dado entre todos los españoles desde el año 2000?</t>
+  </si>
+  <si>
+    <t>1 de cada ___ españoles es de Valencia</t>
+  </si>
+  <si>
+    <t>1 de cada ___ españoles es de Valencia y mide más de 1.90 metros</t>
+  </si>
+  <si>
+    <t>1 de cada ___ españoles es de Valencia y mide más de 1.90 metros y tiene exactamente 20 años</t>
+  </si>
+  <si>
+    <t>1 de cada ___ españoles es de Valencia y mide más de 1.90 metros y tiene exactamente 20 años y su nombre empieza por A</t>
+  </si>
+  <si>
+    <t>¿Cuántos minutos tardas en leer un periódico entero?</t>
+  </si>
+  <si>
+    <t>¿Cuántas horas tuvo el siglo XX?</t>
+  </si>
+  <si>
+    <t>¿Cuántos minutos funciona un coche medio en España antes de acabar en el desguace?</t>
   </si>
   <si>
     <t>¿Cuántas horas de Netflix han visto entre todos los españoles entre 2020 y 2025?</t>
   </si>
   <si>
-    <t>¿Cuántos kilómetros de línea puede dibujar un bolígrafo BIC estándar antes de gastarse?</t>
-  </si>
-  <si>
-    <t>¿Cuántos metros de papel higiénico sin usar hay en un bloque de 10 casas?</t>
-  </si>
-  <si>
-    <t>¿Cuántos pasos darías para cruzar españa de arriba abajo?</t>
-  </si>
-  <si>
-    <t>¿Cuántos pasos da un escarabajo para cruzar españa de arriba abajo?</t>
+    <t>¿Cuántos pasos daría el rey Felipe para cruzar España de arriba abajo?</t>
+  </si>
+  <si>
+    <t>¿Cuántas monedas de un euro tienes que poner haciendo una torre para llegar a lo alto de la torre Eiffel?</t>
+  </si>
+  <si>
+    <t>¿Cuántos metros miden todos los pelos de Rosalía puestos uno detrás de otro?</t>
+  </si>
+  <si>
+    <t>¿Si desenrollaras todo el papel higiénico que consumen los españoles en un año, cuántas veces podrías cubrir el trayecto de Madrid a Barcelona?</t>
   </si>
   <si>
     <t>¿Cuántos granos de arroz caben en una botella de vino?</t>
@@ -117,22 +118,31 @@
     <t>¿Cuántas bolas de pingpong para llenar una piscina olímpica?</t>
   </si>
   <si>
-    <t>¿Cuántos litros de gasolina usaría un coche para llegar hasta la luna?</t>
+    <t>¿Cuántos estadios como el Bernabéu podrías cubrir con todo el cartón papel y cartón que se tira desde las casas de los españoles?</t>
   </si>
   <si>
     <t>¿Cuántos kilos pesan entre todos los españoles?</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>¿Cuántos kilos pesa la Puerta de Alcalá?</t>
-  </si>
-  <si>
-    <t>¿Cuál es el peso total de la atmósfera terrestre?</t>
-  </si>
-  <si>
-    <t>¿Cuál es el presupuesto anual de limpieza de Madrid?</t>
+    <t>¿Cuántos kilos pesan entre todos los teléfonos móviles de España?</t>
+  </si>
+  <si>
+    <t>¿Cuánto pesa la Puerta de Alcalá?</t>
+  </si>
+  <si>
+    <t>¿Cuántos kilos pesan entre todos los coches que pasan por la Cibeles entre las 10 y las 11am un lunes?</t>
+  </si>
+  <si>
+    <t>¿Cuánto dinero se gasta al año una persona que compra un café diario en un bar de Alcorcón cada mañana?</t>
+  </si>
+  <si>
+    <t>¿Cuánto dinero suman todos los coches que se han vendido en España en 2025?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el valor total de todos los iPhone que están funcionando ahora mismo en el mundo?</t>
+  </si>
+  <si>
+    <t>¿Cuánto cuesta mantener encendidas todas las farolas de Madrid durante una noche?</t>
   </si>
   <si>
     <t>test</t>
@@ -154,6 +164,15 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>26 enero 2026</t>
   </si>
 </sst>
 </file>
@@ -188,12 +207,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -202,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -211,6 +236,13 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -233,6 +265,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -700,361 +736,536 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>1.0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>2.0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>3.0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>4.0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>1.0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>2.0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>3.0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>4.0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>1.0</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>2.0</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>3.0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>4.0</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>1.0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>2.0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>3.0</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>4.0</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>1.0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>2.0</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>3.0</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>4.0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>1.0</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>2.0</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>3.0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>4.0</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>1.0</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>2.0</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>3.0</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="4">
         <v>4.0</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>1.0</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>36</v>
+      <c r="C30" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>2.0</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>36</v>
+      <c r="C31" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="4">
         <v>3.0</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>39</v>
+      <c r="C32" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="4">
         <v>4.0</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>36</v>
+      <c r="C33" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1073,366 +1284,397 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>42</v>
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>43</v>
+      <c r="A4" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>43</v>
+      <c r="A5" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
+      <c r="A6" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>43</v>
+      <c r="A7" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>43</v>
+      <c r="A8" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>43</v>
+      <c r="A9" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>44</v>
+      <c r="A10" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>44</v>
+      <c r="A11" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>44</v>
+      <c r="A14" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>44</v>
+      <c r="A15" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>44</v>
+      <c r="A16" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>44</v>
+      <c r="A17" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
+      <c r="A18" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>45</v>
+      <c r="A19" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
+      <c r="A20" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>45</v>
+      <c r="A21" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="s">
-        <v>45</v>
+      <c r="A24" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>45</v>
+      <c r="A25" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="s">
-        <v>46</v>
+      <c r="A26" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="s">
-        <v>46</v>
+      <c r="A27" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="s">
-        <v>46</v>
+      <c r="A28" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>46</v>
+      <c r="A29" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>46</v>
+      <c r="A30" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>46</v>
+      <c r="A31" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="7">
         <v>3.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="7">
         <v>4.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="7">
         <v>4.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change 'chico' por 'masculino' and update questions
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -112,10 +112,10 @@
     <t>¿Cuántos granos de arroz caben en una botella de vino?</t>
   </si>
   <si>
-    <t>¿Cuántas bolas de pingpong para cubrir el césped del Santiago Bernabéu?</t>
-  </si>
-  <si>
-    <t>¿Cuántas bolas de pingpong para llenar una piscina olímpica?</t>
+    <t>¿Cuántas bolas de pingpong se necesitan para cubrir el césped del Santiago Bernabéu?</t>
+  </si>
+  <si>
+    <t>¿Cuántas bolas de pingpong se necesitan para llenar una piscina olímpica?</t>
   </si>
   <si>
     <t>¿Cuántos estadios como el Bernabéu podrías cubrir con todo el cartón papel y cartón que se tira desde las casas de los españoles?</t>

</xml_diff>

<commit_message>
avances en admin, random question, supabase
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="categories" sheetId="1" r:id="rId5"/>
     <sheet state="visible" name="questions" sheetId="2" r:id="rId6"/>
     <sheet state="visible" name="tests" sheetId="3" r:id="rId7"/>
-    <sheet state="visible" name="version" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="other_questions" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>Categoría</t>
   </si>
@@ -118,7 +118,7 @@
     <t>¿Cuántas bolas de pingpong se necesitan para llenar una piscina olímpica?</t>
   </si>
   <si>
-    <t>¿Cuántos estadios como el Bernabéu podrías cubrir con todo el cartón papel y cartón que se tira desde las casas de los españoles?</t>
+    <t>¿Cuántos estadios como el Bernabéu podrías cubrir con todo el papel y cartón que usamos desde los hogares de los españoles?</t>
   </si>
   <si>
     <t>¿Cuántos kilos pesan entre todos los españoles?</t>
@@ -166,13 +166,190 @@
     <t>D</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>26 enero 2026</t>
+    <t>id_play_question</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>¿Cuántos folios A4 se necesitan para cubrir por completo la superficie de un campo de fútbol?</t>
+  </si>
+  <si>
+    <t>¿Cuántas gotas de agua hay en una botella estándar de 1,5 litros?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces parpadea una persona de media a lo largo de toda su vida?</t>
+  </si>
+  <si>
+    <t>¿Cuántas hormigas viven actualmente en toda la península ibérica?</t>
+  </si>
+  <si>
+    <t>¿Cuántos pelos tiene un gato doméstico de tamaño medio?</t>
+  </si>
+  <si>
+    <t>¿Cuántos litros de combustible consume un Airbus A380 en un vuelo de Madrid a Nueva York?</t>
+  </si>
+  <si>
+    <t>¿Cuántas pizzas se reparten en Madrid un sábado por la noche entre las 20:00 y las 23:00?</t>
+  </si>
+  <si>
+    <t>¿Cuántas bombillas hay instaladas en el total de los hogares de España?</t>
+  </si>
+  <si>
+    <t>¿Cuántas palabras pronuncia una persona media a lo largo de un día normal?</t>
+  </si>
+  <si>
+    <t>¿Cuántos granos de arena hay en la playa de la Malvarrosa en Valencia?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno de cada _________ españoles ha nacido un 29 de febrero. </t>
+  </si>
+  <si>
+    <t>¿Cuántas calorías quema un corredor de maratón durante los 42 kilómetros de carrera?</t>
+  </si>
+  <si>
+    <t>¿Cuántos mensajes de WhatsApp se envían en todo el mundo durante un solo segundo?</t>
+  </si>
+  <si>
+    <t>¿Cuántas manzanas de tamaño medio se necesitan para llenar el maletero de un coche utilitario?</t>
+  </si>
+  <si>
+    <t>¿Cuántos litros de leche produce una vaca a lo largo de toda su vida productiva?</t>
+  </si>
+  <si>
+    <t>¿Cuántas hormigas comunes serían necesarias para igualar el peso de un elefante africano?</t>
+  </si>
+  <si>
+    <t>¿Cuántos neumáticos de coche se desechan en España cada año?</t>
+  </si>
+  <si>
+    <t>¿Cuántos minutos de video se suben a YouTube cada hora a nivel global?</t>
+  </si>
+  <si>
+    <t>¿Cuántas monedas de 5 céntimos harían falta para pagar el fichaje de un jugador de fútbol de 100 millones de euros?</t>
+  </si>
+  <si>
+    <t>¿Cuántos kilómetros totales recorre una abeja para producir un solo kilo de miel?</t>
+  </si>
+  <si>
+    <t>¿Cuántos árboles hay plantados en el Parque del Retiro de Madrid?</t>
+  </si>
+  <si>
+    <t>¿Cuántas patatas fritas de bolsa se consumen en los cines de España durante el fin de semana de un gran estreno?</t>
+  </si>
+  <si>
+    <t>¿Cuántas latas de refresco se reciclan en Europa en un día cualquiera?</t>
+  </si>
+  <si>
+    <t>¿Cuántas células tiene el cuerpo de un bebé recién nacido?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno de cada _________ habitantes del mundo vive actualmente en China o en la India. </t>
+  </si>
+  <si>
+    <t>¿Cuántas gotas de lluvia caen sobre una ciudad del tamaño de Sevilla durante una tormenta de 10 minutos?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces cabe el volumen de la Luna dentro del volumen de la Tierra?</t>
+  </si>
+  <si>
+    <t>¿Cuántos cigarrillos se fuman en España en un solo día de diario?</t>
+  </si>
+  <si>
+    <t>¿Cuántos metros de hilo dental usa una persona media si se limpia los dientes cada noche de su vida?</t>
+  </si>
+  <si>
+    <t>¿Cuántos globos de helio estándar se necesitarían para levantar del suelo a una persona de 70 kg?</t>
+  </si>
+  <si>
+    <t>¿Cuántas horas de sueño acumuladas tiene una persona al cumplir los 80 años?</t>
+  </si>
+  <si>
+    <t>¿Cuántas piezas de LEGO existen actualmente en el mundo (fabricadas desde su inicio)?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces late el corazón de un ratón de campo en un solo minuto?</t>
+  </si>
+  <si>
+    <t>¿Cuántos litros de agua se evaporan de una piscina olímpica en un día caluroso de agosto?</t>
+  </si>
+  <si>
+    <t>¿Cuántas fotos digitales hay guardadas en la nube por cada habitante del planeta?</t>
+  </si>
+  <si>
+    <t>¿Cuántas baldosas hay en las aceras de una calle principal de 1 kilómetro de largo?</t>
+  </si>
+  <si>
+    <t>¿Cuántas abejas viven en una colmena típica durante la primavera?</t>
+  </si>
+  <si>
+    <t>¿Cuántas tazas de té se beben en el Reino Unido durante una tarde de domingo?</t>
+  </si>
+  <si>
+    <t>¿Cuántos pasos hay que dar de media para subir al Everest partiendo desde el campamento base?</t>
+  </si>
+  <si>
+    <t>¿Cuántos tornillos y remaches tiene un avión Boeing 747?</t>
+  </si>
+  <si>
+    <t>¿Cuántas búsquedas en Google se realizan desde España durante los 90 minutos de una final de Champions?</t>
+  </si>
+  <si>
+    <t>¿Cuántas tarjetas de crédito caben (en volumen) dentro de una cabina telefónica clásica?</t>
+  </si>
+  <si>
+    <t>¿Cuántos átomos de hidrógeno hay en un vaso de agua de 200 ml?</t>
+  </si>
+  <si>
+    <t>¿Cuántos kilos de basura genera un festival de música multitudinario durante tres días?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces se podría escribir "El Quijote" completo con la tinta de un bolígrafo BIC convencional?</t>
+  </si>
+  <si>
+    <t>¿Cuántas moscas hay en una granja de vacas de tamaño medio en verano?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno de cada _________ coches que circulan por Madrid es de color blanco. </t>
+  </si>
+  <si>
+    <t>¿Cuántos kilómetros de vasos de plástico se formarían si pusiéramos en fila todos los usados en un gran concierto?</t>
+  </si>
+  <si>
+    <t>¿Cuántas respiraciones da un perro de raza media a lo largo de sus 12 años de vida?</t>
+  </si>
+  <si>
+    <t>¿Cuántos paneles solares se necesitarían para cubrir toda la demanda eléctrica de España?</t>
+  </si>
+  <si>
+    <t>¿Cuántos litros de pintura se necesitaron para pintar el exterior de la Casa Blanca?</t>
+  </si>
+  <si>
+    <t>¿Cuántas personas están volando en un avión en este preciso instante en todo el planeta?</t>
+  </si>
+  <si>
+    <t>¿Cuántas palomitas de maíz caben en el habitáculo de un autobús escolar?</t>
+  </si>
+  <si>
+    <t>¿Cuántos granos de azúcar hay en un sobre individual de 8 gramos?</t>
+  </si>
+  <si>
+    <t>¿Cuántos metros crece el pelo de toda la población de una ciudad de 100.000 habitantes en un mes?</t>
+  </si>
+  <si>
+    <t>¿Cuántas llaves de casa hay perdidas u olvidadas en el fondo del mar?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces se ha reproducido el video más visto de YouTube por cada persona viva en la Tierra?</t>
+  </si>
+  <si>
+    <t>¿Cuántas veces daría la vuelta al mundo el cableado eléctrico de una ciudad como Barcelona?</t>
+  </si>
+  <si>
+    <t>¿Cuántos libros físicos hay en todas las bibliotecas públicas de España juntas?</t>
+  </si>
+  <si>
+    <t>¿Cuántas hamburguesas vende McDonald's en todo el mundo en un solo minuto?</t>
   </si>
 </sst>
 </file>
@@ -1660,6 +1837,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="16.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
@@ -1671,10 +1851,482 @@
     </row>
     <row r="2">
       <c r="A2" s="7">
-        <v>1.0</v>
+        <v>101.0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7">
+        <v>103.0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7">
+        <v>105.0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7">
+        <v>106.0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7">
+        <v>107.0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7">
+        <v>108.0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7">
+        <v>109.0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7">
+        <v>110.0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7">
+        <v>111.0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7">
+        <v>112.0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7">
+        <v>113.0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7">
+        <v>114.0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7">
+        <v>115.0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7">
+        <v>116.0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7">
+        <v>117.0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7">
+        <v>118.0</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7">
+        <v>119.0</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7">
+        <v>120.0</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7">
+        <v>121.0</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7">
+        <v>122.0</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7">
+        <v>123.0</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7">
+        <v>124.0</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7">
+        <v>125.0</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7">
+        <v>126.0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7">
+        <v>127.0</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7">
+        <v>128.0</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7">
+        <v>129.0</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7">
+        <v>130.0</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7">
+        <v>131.0</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7">
+        <v>132.0</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7">
+        <v>133.0</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7">
+        <v>134.0</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7">
+        <v>135.0</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="7">
+        <v>136.0</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="7">
+        <v>137.0</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7">
+        <v>138.0</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="7">
+        <v>139.0</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="7">
+        <v>140.0</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="7">
+        <v>141.0</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7">
+        <v>142.0</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="7">
+        <v>143.0</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7">
+        <v>144.0</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="7">
+        <v>145.0</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7">
+        <v>146.0</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7">
+        <v>147.0</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7">
+        <v>148.0</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7">
+        <v>149.0</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7">
+        <v>150.0</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="7">
+        <v>151.0</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7">
+        <v>152.0</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="7">
+        <v>153.0</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="7">
+        <v>154.0</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7">
+        <v>155.0</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7">
+        <v>156.0</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7">
+        <v>157.0</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7">
+        <v>158.0</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7">
+        <v>159.0</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7">
+        <v>160.0</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>